<commit_message>
Sensor BOM minor change
</commit_message>
<xml_diff>
--- a/PCB/OxFloodNet_Sensor_BOM.xlsx
+++ b/PCB/OxFloodNet_Sensor_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="BOM V3.1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
   <si>
     <t>Oxford Flood Network Sensor: Bill of materials</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Screwfix</t>
   </si>
   <si>
-    <t>PCB, V3.0</t>
-  </si>
-  <si>
     <t>thinginnovations.com</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>ANT-900MR</t>
   </si>
   <si>
-    <t>pcb1</t>
-  </si>
-  <si>
     <t>2mm Heatshrink tubing, 5cm</t>
   </si>
   <si>
@@ -232,9 +226,6 @@
     <t>1x7W Right Angle Header pins</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>2356134 (2x12W, cut down)</t>
   </si>
   <si>
@@ -247,9 +238,6 @@
     <t>100nF Ceramic multilayer</t>
   </si>
   <si>
-    <t>Unit Cost</t>
-  </si>
-  <si>
     <t>Technobots Online</t>
   </si>
   <si>
@@ -298,12 +286,6 @@
     <t>2xAA</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Cost exclude VAT</t>
-  </si>
-  <si>
     <t xml:space="preserve">IP55 Enclosure Grey 85 x 75 x 65mm. </t>
   </si>
   <si>
@@ -317,16 +299,16 @@
   </si>
   <si>
     <t>Cost for guidance only</t>
+  </si>
+  <si>
+    <t>PCB, V3.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="17">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,12 +372,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF111111"/>
-      <name val="Lucida Sans Unicode"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="10"/>
@@ -419,21 +395,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="14"/>
       <color theme="1"/>
@@ -450,7 +411,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,8 +436,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -530,40 +509,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -599,19 +548,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -635,51 +571,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -689,67 +586,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1055,73 +939,55 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="35.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="23.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="23.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="18.75">
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="18">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="48">
-        <f>SUM(A28,IF(C3="Yes",A34,0),IF(C4="3.6V Tadiran",A38,A43))</f>
-        <v>110.54000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1">
+        <v>53</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="15.75" customHeight="1">
       <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="28"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="18.75">
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1"/>
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="18">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -1137,43 +1003,30 @@
       <c r="E6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="4" customFormat="1">
-      <c r="A7" s="10" t="s">
-        <v>42</v>
+    </row>
+    <row r="7" spans="1:5" s="4" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="G7" s="15">
-        <f>C7*F7</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="11" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
@@ -1181,23 +1034,16 @@
       <c r="D8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="33">
         <v>2309020</v>
       </c>
-      <c r="F8" s="23">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="G8" s="15">
-        <f t="shared" ref="G8:G27" si="0">C8*F8</f>
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="11" t="s">
-        <v>53</v>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -1205,23 +1051,16 @@
       <c r="D9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="33">
         <v>1144614</v>
       </c>
-      <c r="F9" s="24">
-        <v>0.2</v>
-      </c>
-      <c r="G9" s="15">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="11" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
@@ -1229,23 +1068,16 @@
       <c r="D10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="34">
         <v>2356177</v>
       </c>
-      <c r="F10" s="25">
-        <v>0.22</v>
-      </c>
-      <c r="G10" s="15">
-        <f t="shared" si="0"/>
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="11" t="s">
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
@@ -1253,23 +1085,16 @@
       <c r="D11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="34">
         <v>1098033</v>
       </c>
-      <c r="F11" s="25">
-        <v>0.52</v>
-      </c>
-      <c r="G11" s="15">
-        <f t="shared" si="0"/>
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="11" t="s">
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
@@ -1277,23 +1102,16 @@
       <c r="D12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="34">
         <v>2356180</v>
       </c>
-      <c r="F12" s="25">
-        <v>0.51</v>
-      </c>
-      <c r="G12" s="15">
-        <f t="shared" si="0"/>
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="11" t="s">
-        <v>51</v>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C13" s="6">
         <v>1</v>
@@ -1301,23 +1119,16 @@
       <c r="D13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="25">
-        <v>0.73</v>
-      </c>
-      <c r="G13" s="15">
-        <f>C13*F13</f>
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="11" t="s">
+      <c r="E13" s="34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C14" s="6">
         <v>1</v>
@@ -1325,23 +1136,16 @@
       <c r="D14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="34">
         <v>1187948</v>
       </c>
-      <c r="F14" s="25">
-        <v>4.13</v>
-      </c>
-      <c r="G14" s="15">
-        <f t="shared" si="0"/>
-        <v>4.13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="11" t="s">
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
@@ -1349,21 +1153,14 @@
       <c r="D15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="34">
         <v>1098037</v>
       </c>
-      <c r="F15" s="25">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="G15" s="15">
-        <f t="shared" si="0"/>
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="11"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="9"/>
       <c r="B16" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
@@ -1371,19 +1168,12 @@
       <c r="D16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="34">
         <v>2356182</v>
       </c>
-      <c r="F16" s="25">
-        <v>0.65</v>
-      </c>
-      <c r="G16" s="15">
-        <f t="shared" si="0"/>
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="11" t="s">
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1395,23 +1185,16 @@
       <c r="D17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="34">
         <v>9845178</v>
       </c>
-      <c r="F17" s="25">
-        <v>0.09</v>
-      </c>
-      <c r="G17" s="15">
-        <f t="shared" si="0"/>
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="11" t="s">
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
@@ -1419,19 +1202,12 @@
       <c r="D18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="34">
         <v>2329534</v>
       </c>
-      <c r="F18" s="25">
-        <v>0.02</v>
-      </c>
-      <c r="G18" s="15">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="11" t="s">
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1443,19 +1219,12 @@
       <c r="D19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="34">
         <v>1109732</v>
       </c>
-      <c r="F19" s="25">
-        <v>2.08</v>
-      </c>
-      <c r="G19" s="15">
-        <f t="shared" si="0"/>
-        <v>4.16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="11" t="s">
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -1470,20 +1239,13 @@
       <c r="E20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="25">
-        <v>11.66</v>
-      </c>
-      <c r="G20" s="15">
-        <f t="shared" si="0"/>
-        <v>11.66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="11" t="s">
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C21" s="6">
         <v>1</v>
@@ -1494,16 +1256,9 @@
       <c r="E21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="25">
-        <v>64</v>
-      </c>
-      <c r="G21" s="15">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="11"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="9"/>
       <c r="B22" s="6" t="s">
         <v>36</v>
       </c>
@@ -1514,112 +1269,77 @@
         <v>35</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="25">
-        <v>1.73</v>
-      </c>
-      <c r="G22" s="15">
-        <f t="shared" si="0"/>
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="11"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="9"/>
       <c r="B23" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="G23" s="15">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="H23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="11"/>
+        <v>91</v>
+      </c>
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="9"/>
       <c r="B24" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C24" s="6">
         <v>2</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="G24" s="15">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="H24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="11"/>
+        <v>91</v>
+      </c>
+      <c r="F24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="9"/>
       <c r="B25" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" s="6">
         <v>1</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="G25" s="15">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="H25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="11"/>
+        <v>91</v>
+      </c>
+      <c r="F25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="9"/>
       <c r="B26" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="G26" s="15">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="H26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="11"/>
+        <v>91</v>
+      </c>
+      <c r="F26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="9"/>
       <c r="B27" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C27" s="6">
         <v>1</v>
@@ -1628,319 +1348,219 @@
         <v>37</v>
       </c>
       <c r="E27" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="29"/>
+      <c r="B31" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="30">
+        <v>1</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="30">
+        <v>1</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" s="10"/>
+      <c r="J32" s="11"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="30">
+        <v>1</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="24">
+        <v>2</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="23"/>
+      <c r="B37" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="24">
+        <v>1</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="12"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="25"/>
+      <c r="B40" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="26">
+        <v>1</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="26">
+        <v>1702631</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="25"/>
+      <c r="B41" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="25">
-        <v>2.91</v>
-      </c>
-      <c r="G27" s="15">
-        <f t="shared" si="0"/>
-        <v>2.91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="29">
-        <f>SUM(G7:G27)</f>
-        <v>95.730000000000018</v>
-      </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="31"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="37"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="6">
-        <v>1</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="C41" s="26">
+        <v>1</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="26">
+        <v>1098034</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" customHeight="1">
+      <c r="A42" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="26">
+        <v>1</v>
+      </c>
+      <c r="D42" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="25">
-        <v>1</v>
-      </c>
-      <c r="G30" s="12">
-        <f>C30*F30</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="13"/>
-      <c r="B31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="6">
-        <v>1</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="25">
-        <v>3.33</v>
-      </c>
-      <c r="G31" s="12">
-        <f t="shared" ref="G31:G33" si="1">C31*F31</f>
-        <v>3.33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="6">
-        <v>1</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F32" s="25">
-        <v>1.59</v>
-      </c>
-      <c r="G32" s="15">
-        <f>C32*F32</f>
-        <v>1.59</v>
-      </c>
-      <c r="H32" t="s">
-        <v>79</v>
-      </c>
-      <c r="K32" s="17"/>
-      <c r="L32" s="20"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="6">
-        <v>1</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="26">
-        <v>5</v>
-      </c>
-      <c r="G33" s="12">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="29">
-        <f>SUM(G30:G33)</f>
-        <v>10.92</v>
-      </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="31"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="37"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="6">
-        <v>2</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="G36" s="12">
-        <f>C36*F36</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="11"/>
-      <c r="B37" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="6">
-        <v>1</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="25">
-        <v>3.49</v>
-      </c>
-      <c r="G37" s="12">
-        <f>C37*F37</f>
-        <v>3.49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="32">
-        <f>SUM(G36:G37)</f>
-        <v>3.89</v>
-      </c>
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="34"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="37"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="39"/>
-      <c r="B40" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="40">
-        <v>1</v>
-      </c>
-      <c r="D40" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="40">
-        <v>1702631</v>
-      </c>
-      <c r="F40" s="41">
-        <v>0.99</v>
-      </c>
-      <c r="G40" s="42">
-        <f>C40*F40</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="39"/>
-      <c r="B41" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="40">
-        <v>1</v>
-      </c>
-      <c r="D41" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="40">
-        <v>1098034</v>
-      </c>
-      <c r="F41" s="41">
-        <v>0.78</v>
-      </c>
-      <c r="G41" s="42">
-        <f t="shared" ref="G41:G42" si="2">C41*F41</f>
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1">
-      <c r="A42" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="44" t="s">
+      <c r="E42" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="40">
-        <v>1</v>
-      </c>
-      <c r="D42" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E42" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" s="41">
-        <v>4.16</v>
-      </c>
-      <c r="G42" s="42">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A43" s="45">
-        <f>SUM(G40:G42)</f>
-        <v>5.93</v>
-      </c>
-      <c r="B43" s="46"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="47"/>
+    </row>
+    <row r="43" spans="1:5" ht="15" thickBot="1">
+      <c r="A43" s="21"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A34:G34"/>
+  <mergeCells count="3">
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A29:E29"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
@@ -1963,67 +1583,67 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="17" t="s">
-        <v>58</v>
+      <c r="A1" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="50" t="s">
-        <v>62</v>
+      <c r="B3" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="50" t="s">
-        <v>60</v>
+      <c r="B4" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>39</v>
+        <v>57</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>76</v>
+        <v>71</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="51" t="s">
-        <v>85</v>
+        <v>47</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2048,26 +1668,26 @@
       <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>